<commit_message>
v1.6.4  Passat a fitxer de config .yaml que es editable per humans + bugfixing
</commit_message>
<xml_diff>
--- a/revisio_copies_seguretat_synology_vs1.xlsx
+++ b/revisio_copies_seguretat_synology_vs1.xlsx
@@ -2664,13 +2664,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E54AFD4F-0ED2-448C-BBAF-F648A649256D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2571FAE-F8AF-46B7-ACAD-DF7D44BAE4C5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044E1E34-A84B-4B3A-AA0F-1EF3625900E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9185F38-D610-4085-B5E8-3987A369AA35}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F21474D-5F3D-45A2-B6F7-8A500F529C6A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D56D5AB3-0616-443E-BFE5-7A4F6147E7D0}"/>
 </file>
</xml_diff>

<commit_message>
Millor readme + fix bug #3
</commit_message>
<xml_diff>
--- a/revisio_copies_seguretat_synology_vs1.xlsx
+++ b/revisio_copies_seguretat_synology_vs1.xlsx
@@ -567,7 +567,7 @@
         <v/>
       </c>
       <c r="F3" t="n">
-        <v>1785</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="4">
@@ -594,7 +594,7 @@
         <v/>
       </c>
       <c r="F4" t="n">
-        <v>1785</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="5">
@@ -621,7 +621,7 @@
         <v/>
       </c>
       <c r="F5" t="n">
-        <v>1785</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="6">
@@ -648,7 +648,7 @@
         <v/>
       </c>
       <c r="F6" t="n">
-        <v>1785</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v/>
       </c>
       <c r="F7" t="n">
-        <v>1785</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="8">
@@ -702,7 +702,7 @@
         <v/>
       </c>
       <c r="F8" t="n">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="9">
@@ -729,7 +729,7 @@
         <v/>
       </c>
       <c r="F9" t="n">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="10">
@@ -756,7 +756,7 @@
         <v/>
       </c>
       <c r="F10" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="11">
@@ -783,7 +783,7 @@
         <v/>
       </c>
       <c r="F11" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="12">
@@ -810,7 +810,7 @@
         <v/>
       </c>
       <c r="F12" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="13">
@@ -837,7 +837,7 @@
         <v/>
       </c>
       <c r="F13" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="14">
@@ -864,7 +864,7 @@
         <v/>
       </c>
       <c r="F14" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="15">
@@ -891,7 +891,7 @@
         <v/>
       </c>
       <c r="F15" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="16">
@@ -918,7 +918,7 @@
         <v/>
       </c>
       <c r="F16" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="17">
@@ -945,7 +945,7 @@
         <v/>
       </c>
       <c r="F17" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="18">
@@ -972,7 +972,7 @@
         <v/>
       </c>
       <c r="F18" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="19">
@@ -999,7 +999,7 @@
         <v/>
       </c>
       <c r="F19" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="20">
@@ -1026,7 +1026,7 @@
         <v/>
       </c>
       <c r="F20" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="21">
@@ -1053,7 +1053,7 @@
         <v/>
       </c>
       <c r="F21" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="22">
@@ -1080,7 +1080,7 @@
         <v/>
       </c>
       <c r="F22" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="23">
@@ -1107,7 +1107,7 @@
         <v/>
       </c>
       <c r="F23" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="24">
@@ -1134,7 +1134,7 @@
         <v/>
       </c>
       <c r="F24" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="25">
@@ -1161,7 +1161,7 @@
         <v/>
       </c>
       <c r="F25" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="26">
@@ -1188,7 +1188,7 @@
         <v/>
       </c>
       <c r="F26" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="27">
@@ -1215,7 +1215,7 @@
         <v/>
       </c>
       <c r="F27" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="28">
@@ -1242,7 +1242,7 @@
         <v/>
       </c>
       <c r="F28" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="29">
@@ -1269,7 +1269,7 @@
         <v/>
       </c>
       <c r="F29" t="n">
-        <v>1664</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="30">
@@ -1296,7 +1296,7 @@
         <v/>
       </c>
       <c r="F30" t="n">
-        <v>4757</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="31">
@@ -1323,7 +1323,7 @@
         <v/>
       </c>
       <c r="F31" t="n">
-        <v>4757</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="32">
@@ -1350,7 +1350,7 @@
         <v/>
       </c>
       <c r="F32" t="n">
-        <v>4757</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="33">
@@ -1377,7 +1377,7 @@
         <v/>
       </c>
       <c r="F33" t="n">
-        <v>4757</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="34">
@@ -1404,7 +1404,7 @@
         <v/>
       </c>
       <c r="F34" t="n">
-        <v>4757</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="35">
@@ -1431,7 +1431,7 @@
         <v/>
       </c>
       <c r="F35" t="n">
-        <v>4757</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="36">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AURT0001SV0719</t>
+          <t>SIS0010SV0721</t>
         </is>
       </c>
       <c r="C36">
@@ -1458,7 +1458,7 @@
         <v/>
       </c>
       <c r="F36" t="n">
-        <v>1785</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="37">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PCDOLORS</t>
+          <t>SIS0011SV0721</t>
         </is>
       </c>
       <c r="C37">
@@ -1485,794 +1485,790 @@
         <v/>
       </c>
       <c r="F37" t="n">
-        <v>1785</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sismic</t>
+          <t>TorinoLocal</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PC-USUARI2</t>
+          <t>SERVER1</t>
         </is>
       </c>
       <c r="C38">
-        <f>LOOKUP(2,1/(Sismic!9:9&lt;&gt;""),Sismic!9:9)</f>
+        <f>LOOKUP(2,1/(TorinoLocal!1:1&lt;&gt;""),TorinoLocal!1:1)</f>
         <v/>
       </c>
       <c r="D38">
-        <f>LOOKUP(2,1/(Sismic!11:11&lt;&gt;""),Sismic!11:11)</f>
+        <f>LOOKUP(2,1/(TorinoLocal!3:3&lt;&gt;""),TorinoLocal!3:3)</f>
         <v/>
       </c>
       <c r="E38">
-        <f>LOOKUP(2,1/(Sismic!10:10&lt;&gt;""),Sismic!10:10)</f>
+        <f>LOOKUP(2,1/(TorinoLocal!2:2&lt;&gt;""),TorinoLocal!2:2)</f>
         <v/>
       </c>
       <c r="F38" t="n">
-        <v>1785</v>
+        <v>426</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sismic</t>
+          <t>TorinoLocal</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PCMARC1</t>
+          <t>PCDIRECCIO</t>
         </is>
       </c>
       <c r="C39">
-        <f>LOOKUP(2,1/(Sismic!13:13&lt;&gt;""),Sismic!13:13)</f>
+        <f>LOOKUP(2,1/(TorinoLocal!5:5&lt;&gt;""),TorinoLocal!5:5)</f>
         <v/>
       </c>
       <c r="D39">
-        <f>LOOKUP(2,1/(Sismic!15:15&lt;&gt;""),Sismic!15:15)</f>
+        <f>LOOKUP(2,1/(TorinoLocal!7:7&lt;&gt;""),TorinoLocal!7:7)</f>
         <v/>
       </c>
       <c r="E39">
-        <f>LOOKUP(2,1/(Sismic!14:14&lt;&gt;""),Sismic!14:14)</f>
+        <f>LOOKUP(2,1/(TorinoLocal!6:6&lt;&gt;""),TorinoLocal!6:6)</f>
         <v/>
       </c>
       <c r="F39" t="n">
-        <v>1785</v>
+        <v>426</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sismic</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PCUSUARI3</t>
+          <t>Server235 - TS B1 Nou</t>
         </is>
       </c>
       <c r="C40">
-        <f>LOOKUP(2,1/(Sismic!17:17&lt;&gt;""),Sismic!17:17)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!1:1&lt;&gt;""),TransportsTresserras!1:1)</f>
         <v/>
       </c>
       <c r="D40">
-        <f>LOOKUP(2,1/(Sismic!19:19&lt;&gt;""),Sismic!19:19)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!3:3&lt;&gt;""),TransportsTresserras!3:3)</f>
         <v/>
       </c>
       <c r="E40">
-        <f>LOOKUP(2,1/(Sismic!18:18&lt;&gt;""),Sismic!18:18)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!2:2&lt;&gt;""),TransportsTresserras!2:2)</f>
         <v/>
       </c>
       <c r="F40" t="n">
-        <v>1785</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TallerJoa</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SERVER1</t>
+          <t>Server226</t>
         </is>
       </c>
       <c r="C41">
-        <f>LOOKUP(2,1/(TallerJoa!1:1&lt;&gt;""),TallerJoa!1:1)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!5:5&lt;&gt;""),TransportsTresserras!5:5)</f>
         <v/>
       </c>
       <c r="D41">
-        <f>LOOKUP(2,1/(TallerJoa!3:3&lt;&gt;""),TallerJoa!3:3)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!7:7&lt;&gt;""),TransportsTresserras!7:7)</f>
         <v/>
       </c>
       <c r="E41">
-        <f>LOOKUP(2,1/(TallerJoa!2:2&lt;&gt;""),TallerJoa!2:2)</f>
-        <v/>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Fallo en la conexio</t>
-        </is>
+        <f>LOOKUP(2,1/(TransportsTresserras!6:6&lt;&gt;""),TransportsTresserras!6:6)</f>
+        <v/>
+      </c>
+      <c r="F41" t="n">
+        <v>7177</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TallerJoa</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PCDIRECCIO</t>
+          <t>PcVirtual1 - planella</t>
         </is>
       </c>
       <c r="C42">
-        <f>LOOKUP(2,1/(TallerJoa!5:5&lt;&gt;""),TallerJoa!5:5)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!9:9&lt;&gt;""),TransportsTresserras!9:9)</f>
         <v/>
       </c>
       <c r="D42">
-        <f>LOOKUP(2,1/(TallerJoa!7:7&lt;&gt;""),TallerJoa!7:7)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!11:11&lt;&gt;""),TransportsTresserras!11:11)</f>
         <v/>
       </c>
       <c r="E42">
-        <f>LOOKUP(2,1/(TallerJoa!6:6&lt;&gt;""),TallerJoa!6:6)</f>
-        <v/>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Fallo en la conexio</t>
-        </is>
+        <f>LOOKUP(2,1/(TransportsTresserras!10:10&lt;&gt;""),TransportsTresserras!10:10)</f>
+        <v/>
+      </c>
+      <c r="F42" t="n">
+        <v>7177</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Server235 - TS B1 Nou</t>
+          <t>Server215 - KSC</t>
         </is>
       </c>
       <c r="C43">
-        <f>LOOKUP(2,1/(TorinoLocal!1:1&lt;&gt;""),TorinoLocal!1:1)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!13:13&lt;&gt;""),TransportsTresserras!13:13)</f>
         <v/>
       </c>
       <c r="D43">
-        <f>LOOKUP(2,1/(TorinoLocal!3:3&lt;&gt;""),TorinoLocal!3:3)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!15:15&lt;&gt;""),TransportsTresserras!15:15)</f>
         <v/>
       </c>
       <c r="E43">
-        <f>LOOKUP(2,1/(TorinoLocal!2:2&lt;&gt;""),TorinoLocal!2:2)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!14:14&lt;&gt;""),TransportsTresserras!14:14)</f>
         <v/>
       </c>
       <c r="F43" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Server226</t>
+          <t>Server219 - TS</t>
         </is>
       </c>
       <c r="C44">
-        <f>LOOKUP(2,1/(TorinoLocal!5:5&lt;&gt;""),TorinoLocal!5:5)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!17:17&lt;&gt;""),TransportsTresserras!17:17)</f>
         <v/>
       </c>
       <c r="D44">
-        <f>LOOKUP(2,1/(TorinoLocal!7:7&lt;&gt;""),TorinoLocal!7:7)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!19:19&lt;&gt;""),TransportsTresserras!19:19)</f>
         <v/>
       </c>
       <c r="E44">
-        <f>LOOKUP(2,1/(TorinoLocal!6:6&lt;&gt;""),TorinoLocal!6:6)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!18:18&lt;&gt;""),TransportsTresserras!18:18)</f>
         <v/>
       </c>
       <c r="F44" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>PcVirtual1 - planella</t>
+          <t>Server220 - Web</t>
         </is>
       </c>
       <c r="C45">
-        <f>LOOKUP(2,1/(TorinoLocal!9:9&lt;&gt;""),TorinoLocal!9:9)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!21:21&lt;&gt;""),TransportsTresserras!21:21)</f>
         <v/>
       </c>
       <c r="D45">
-        <f>LOOKUP(2,1/(TorinoLocal!11:11&lt;&gt;""),TorinoLocal!11:11)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!23:23&lt;&gt;""),TransportsTresserras!23:23)</f>
         <v/>
       </c>
       <c r="E45">
-        <f>LOOKUP(2,1/(TorinoLocal!10:10&lt;&gt;""),TorinoLocal!10:10)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!22:22&lt;&gt;""),TransportsTresserras!22:22)</f>
         <v/>
       </c>
       <c r="F45" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Server215 - KSC</t>
+          <t>Server236 - Qlik</t>
         </is>
       </c>
       <c r="C46">
-        <f>LOOKUP(2,1/(TorinoLocal!13:13&lt;&gt;""),TorinoLocal!13:13)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!25:25&lt;&gt;""),TransportsTresserras!25:25)</f>
         <v/>
       </c>
       <c r="D46">
-        <f>LOOKUP(2,1/(TorinoLocal!15:15&lt;&gt;""),TorinoLocal!15:15)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!27:27&lt;&gt;""),TransportsTresserras!27:27)</f>
         <v/>
       </c>
       <c r="E46">
-        <f>LOOKUP(2,1/(TorinoLocal!14:14&lt;&gt;""),TorinoLocal!14:14)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!26:26&lt;&gt;""),TransportsTresserras!26:26)</f>
         <v/>
       </c>
       <c r="F46" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Server219 - TS</t>
+          <t>pcvirutal09_win10 - EDI</t>
         </is>
       </c>
       <c r="C47">
-        <f>LOOKUP(2,1/(TorinoLocal!17:17&lt;&gt;""),TorinoLocal!17:17)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!29:29&lt;&gt;""),TransportsTresserras!29:29)</f>
         <v/>
       </c>
       <c r="D47">
-        <f>LOOKUP(2,1/(TorinoLocal!19:19&lt;&gt;""),TorinoLocal!19:19)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!31:31&lt;&gt;""),TransportsTresserras!31:31)</f>
         <v/>
       </c>
       <c r="E47">
-        <f>LOOKUP(2,1/(TorinoLocal!18:18&lt;&gt;""),TorinoLocal!18:18)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!30:30&lt;&gt;""),TransportsTresserras!30:30)</f>
         <v/>
       </c>
       <c r="F47" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Server220 - Web</t>
+          <t>SERVER203 - Progress</t>
         </is>
       </c>
       <c r="C48">
-        <f>LOOKUP(2,1/(TorinoLocal!21:21&lt;&gt;""),TorinoLocal!21:21)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!33:33&lt;&gt;""),TransportsTresserras!33:33)</f>
         <v/>
       </c>
       <c r="D48">
-        <f>LOOKUP(2,1/(TorinoLocal!23:23&lt;&gt;""),TorinoLocal!23:23)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!35:35&lt;&gt;""),TransportsTresserras!35:35)</f>
         <v/>
       </c>
       <c r="E48">
-        <f>LOOKUP(2,1/(TorinoLocal!22:22&lt;&gt;""),TorinoLocal!22:22)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!34:34&lt;&gt;""),TransportsTresserras!34:34)</f>
         <v/>
       </c>
       <c r="F48" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Server236 - Qlik</t>
+          <t>Server221- Aduana</t>
         </is>
       </c>
       <c r="C49">
-        <f>LOOKUP(2,1/(TorinoLocal!25:25&lt;&gt;""),TorinoLocal!25:25)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!37:37&lt;&gt;""),TransportsTresserras!37:37)</f>
         <v/>
       </c>
       <c r="D49">
-        <f>LOOKUP(2,1/(TorinoLocal!27:27&lt;&gt;""),TorinoLocal!27:27)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!39:39&lt;&gt;""),TransportsTresserras!39:39)</f>
         <v/>
       </c>
       <c r="E49">
-        <f>LOOKUP(2,1/(TorinoLocal!26:26&lt;&gt;""),TorinoLocal!26:26)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!38:38&lt;&gt;""),TransportsTresserras!38:38)</f>
         <v/>
       </c>
       <c r="F49" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>pcvirutal09_win10 - EDI</t>
+          <t>Server223</t>
         </is>
       </c>
       <c r="C50">
-        <f>LOOKUP(2,1/(TorinoLocal!29:29&lt;&gt;""),TorinoLocal!29:29)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!41:41&lt;&gt;""),TransportsTresserras!41:41)</f>
         <v/>
       </c>
       <c r="D50">
-        <f>LOOKUP(2,1/(TorinoLocal!31:31&lt;&gt;""),TorinoLocal!31:31)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!43:43&lt;&gt;""),TransportsTresserras!43:43)</f>
         <v/>
       </c>
       <c r="E50">
-        <f>LOOKUP(2,1/(TorinoLocal!30:30&lt;&gt;""),TorinoLocal!30:30)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!42:42&lt;&gt;""),TransportsTresserras!42:42)</f>
         <v/>
       </c>
       <c r="F50" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SERVER203 - Progress</t>
+          <t>Server224 - AD2k12 - restored</t>
         </is>
       </c>
       <c r="C51">
-        <f>LOOKUP(2,1/(TorinoLocal!33:33&lt;&gt;""),TorinoLocal!33:33)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!45:45&lt;&gt;""),TransportsTresserras!45:45)</f>
         <v/>
       </c>
       <c r="D51">
-        <f>LOOKUP(2,1/(TorinoLocal!35:35&lt;&gt;""),TorinoLocal!35:35)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!47:47&lt;&gt;""),TransportsTresserras!47:47)</f>
         <v/>
       </c>
       <c r="E51">
-        <f>LOOKUP(2,1/(TorinoLocal!34:34&lt;&gt;""),TorinoLocal!34:34)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!46:46&lt;&gt;""),TransportsTresserras!46:46)</f>
         <v/>
       </c>
       <c r="F51" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Server221- Aduana</t>
+          <t>Server228 - GMagat</t>
         </is>
       </c>
       <c r="C52">
-        <f>LOOKUP(2,1/(TorinoLocal!37:37&lt;&gt;""),TorinoLocal!37:37)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!49:49&lt;&gt;""),TransportsTresserras!49:49)</f>
         <v/>
       </c>
       <c r="D52">
-        <f>LOOKUP(2,1/(TorinoLocal!39:39&lt;&gt;""),TorinoLocal!39:39)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!51:51&lt;&gt;""),TransportsTresserras!51:51)</f>
         <v/>
       </c>
       <c r="E52">
-        <f>LOOKUP(2,1/(TorinoLocal!38:38&lt;&gt;""),TorinoLocal!38:38)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!50:50&lt;&gt;""),TransportsTresserras!50:50)</f>
         <v/>
       </c>
       <c r="F52" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Server223</t>
+          <t>Server229 - IP6</t>
         </is>
       </c>
       <c r="C53">
-        <f>LOOKUP(2,1/(TorinoLocal!41:41&lt;&gt;""),TorinoLocal!41:41)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!53:53&lt;&gt;""),TransportsTresserras!53:53)</f>
         <v/>
       </c>
       <c r="D53">
-        <f>LOOKUP(2,1/(TorinoLocal!43:43&lt;&gt;""),TorinoLocal!43:43)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!55:55&lt;&gt;""),TransportsTresserras!55:55)</f>
         <v/>
       </c>
       <c r="E53">
-        <f>LOOKUP(2,1/(TorinoLocal!42:42&lt;&gt;""),TorinoLocal!42:42)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!54:54&lt;&gt;""),TransportsTresserras!54:54)</f>
         <v/>
       </c>
       <c r="F53" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Server224 - AD2k12 - restored</t>
+          <t>Server238 - InterCompany</t>
         </is>
       </c>
       <c r="C54">
-        <f>LOOKUP(2,1/(TorinoLocal!45:45&lt;&gt;""),TorinoLocal!45:45)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!57:57&lt;&gt;""),TransportsTresserras!57:57)</f>
         <v/>
       </c>
       <c r="D54">
-        <f>LOOKUP(2,1/(TorinoLocal!47:47&lt;&gt;""),TorinoLocal!47:47)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!59:59&lt;&gt;""),TransportsTresserras!59:59)</f>
         <v/>
       </c>
       <c r="E54">
-        <f>LOOKUP(2,1/(TorinoLocal!46:46&lt;&gt;""),TorinoLocal!46:46)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!58:58&lt;&gt;""),TransportsTresserras!58:58)</f>
         <v/>
       </c>
       <c r="F54" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Server228 - GMagat</t>
+          <t>Server244 - Dades</t>
         </is>
       </c>
       <c r="C55">
-        <f>LOOKUP(2,1/(TorinoLocal!49:49&lt;&gt;""),TorinoLocal!49:49)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!61:61&lt;&gt;""),TransportsTresserras!61:61)</f>
         <v/>
       </c>
       <c r="D55">
-        <f>LOOKUP(2,1/(TorinoLocal!51:51&lt;&gt;""),TorinoLocal!51:51)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!63:63&lt;&gt;""),TransportsTresserras!63:63)</f>
         <v/>
       </c>
       <c r="E55">
-        <f>LOOKUP(2,1/(TorinoLocal!50:50&lt;&gt;""),TorinoLocal!50:50)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!62:62&lt;&gt;""),TransportsTresserras!62:62)</f>
         <v/>
       </c>
       <c r="F55" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Server229 - IP6</t>
+          <t>pcvirtual08_win7 - Spiceworks</t>
         </is>
       </c>
       <c r="C56">
-        <f>LOOKUP(2,1/(TorinoLocal!53:53&lt;&gt;""),TorinoLocal!53:53)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!65:65&lt;&gt;""),TransportsTresserras!65:65)</f>
         <v/>
       </c>
       <c r="D56">
-        <f>LOOKUP(2,1/(TorinoLocal!55:55&lt;&gt;""),TorinoLocal!55:55)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!67:67&lt;&gt;""),TransportsTresserras!67:67)</f>
         <v/>
       </c>
       <c r="E56">
-        <f>LOOKUP(2,1/(TorinoLocal!54:54&lt;&gt;""),TorinoLocal!54:54)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!66:66&lt;&gt;""),TransportsTresserras!66:66)</f>
         <v/>
       </c>
       <c r="F56" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Server238 - InterCompany</t>
+          <t>Server227</t>
         </is>
       </c>
       <c r="C57">
-        <f>LOOKUP(2,1/(TorinoLocal!57:57&lt;&gt;""),TorinoLocal!57:57)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!69:69&lt;&gt;""),TransportsTresserras!69:69)</f>
         <v/>
       </c>
       <c r="D57">
-        <f>LOOKUP(2,1/(TorinoLocal!59:59&lt;&gt;""),TorinoLocal!59:59)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!71:71&lt;&gt;""),TransportsTresserras!71:71)</f>
         <v/>
       </c>
       <c r="E57">
-        <f>LOOKUP(2,1/(TorinoLocal!58:58&lt;&gt;""),TorinoLocal!58:58)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!70:70&lt;&gt;""),TransportsTresserras!70:70)</f>
         <v/>
       </c>
       <c r="F57" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Server244 - Dades</t>
+          <t>ServerBCN220 - dcserver BCN</t>
         </is>
       </c>
       <c r="C58">
-        <f>LOOKUP(2,1/(TorinoLocal!61:61&lt;&gt;""),TorinoLocal!61:61)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!73:73&lt;&gt;""),TransportsTresserras!73:73)</f>
         <v/>
       </c>
       <c r="D58">
-        <f>LOOKUP(2,1/(TorinoLocal!63:63&lt;&gt;""),TorinoLocal!63:63)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!75:75&lt;&gt;""),TransportsTresserras!75:75)</f>
         <v/>
       </c>
       <c r="E58">
-        <f>LOOKUP(2,1/(TorinoLocal!62:62&lt;&gt;""),TorinoLocal!62:62)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!74:74&lt;&gt;""),TransportsTresserras!74:74)</f>
         <v/>
       </c>
       <c r="F58" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>pcvirtual08_win7 - Spiceworks</t>
+          <t>SERVER208</t>
         </is>
       </c>
       <c r="C59">
-        <f>LOOKUP(2,1/(TorinoLocal!65:65&lt;&gt;""),TorinoLocal!65:65)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!77:77&lt;&gt;""),TransportsTresserras!77:77)</f>
         <v/>
       </c>
       <c r="D59">
-        <f>LOOKUP(2,1/(TorinoLocal!67:67&lt;&gt;""),TorinoLocal!67:67)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!79:79&lt;&gt;""),TransportsTresserras!79:79)</f>
         <v/>
       </c>
       <c r="E59">
-        <f>LOOKUP(2,1/(TorinoLocal!66:66&lt;&gt;""),TorinoLocal!66:66)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!78:78&lt;&gt;""),TransportsTresserras!78:78)</f>
         <v/>
       </c>
       <c r="F59" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Server227</t>
+          <t>SERVER222</t>
         </is>
       </c>
       <c r="C60">
-        <f>LOOKUP(2,1/(TorinoLocal!69:69&lt;&gt;""),TorinoLocal!69:69)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!81:81&lt;&gt;""),TransportsTresserras!81:81)</f>
         <v/>
       </c>
       <c r="D60">
-        <f>LOOKUP(2,1/(TorinoLocal!71:71&lt;&gt;""),TorinoLocal!71:71)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!83:83&lt;&gt;""),TransportsTresserras!83:83)</f>
         <v/>
       </c>
       <c r="E60">
-        <f>LOOKUP(2,1/(TorinoLocal!70:70&lt;&gt;""),TorinoLocal!70:70)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!82:82&lt;&gt;""),TransportsTresserras!82:82)</f>
         <v/>
       </c>
       <c r="F60" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ServerBCN220 - dcserver BCN</t>
+          <t>Server200-VCenter</t>
         </is>
       </c>
       <c r="C61">
-        <f>LOOKUP(2,1/(TorinoLocal!73:73&lt;&gt;""),TorinoLocal!73:73)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!85:85&lt;&gt;""),TransportsTresserras!85:85)</f>
         <v/>
       </c>
       <c r="D61">
-        <f>LOOKUP(2,1/(TorinoLocal!75:75&lt;&gt;""),TorinoLocal!75:75)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!87:87&lt;&gt;""),TransportsTresserras!87:87)</f>
         <v/>
       </c>
       <c r="E61">
-        <f>LOOKUP(2,1/(TorinoLocal!74:74&lt;&gt;""),TorinoLocal!74:74)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!86:86&lt;&gt;""),TransportsTresserras!86:86)</f>
         <v/>
       </c>
       <c r="F61" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>SERVER208</t>
+          <t>server251 - Unifi controller</t>
         </is>
       </c>
       <c r="C62">
-        <f>LOOKUP(2,1/(TorinoLocal!77:77&lt;&gt;""),TorinoLocal!77:77)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!89:89&lt;&gt;""),TransportsTresserras!89:89)</f>
         <v/>
       </c>
       <c r="D62">
-        <f>LOOKUP(2,1/(TorinoLocal!79:79&lt;&gt;""),TorinoLocal!79:79)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!91:91&lt;&gt;""),TransportsTresserras!91:91)</f>
         <v/>
       </c>
       <c r="E62">
-        <f>LOOKUP(2,1/(TorinoLocal!78:78&lt;&gt;""),TorinoLocal!78:78)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!90:90&lt;&gt;""),TransportsTresserras!90:90)</f>
         <v/>
       </c>
       <c r="F62" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SERVER222</t>
+          <t>Server237 - SAPupdate (1)</t>
         </is>
       </c>
       <c r="C63">
-        <f>LOOKUP(2,1/(TorinoLocal!81:81&lt;&gt;""),TorinoLocal!81:81)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!93:93&lt;&gt;""),TransportsTresserras!93:93)</f>
         <v/>
       </c>
       <c r="D63">
-        <f>LOOKUP(2,1/(TorinoLocal!83:83&lt;&gt;""),TorinoLocal!83:83)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!95:95&lt;&gt;""),TransportsTresserras!95:95)</f>
         <v/>
       </c>
       <c r="E63">
-        <f>LOOKUP(2,1/(TorinoLocal!82:82&lt;&gt;""),TorinoLocal!82:82)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!94:94&lt;&gt;""),TransportsTresserras!94:94)</f>
         <v/>
       </c>
       <c r="F63" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Server200-VCenter</t>
+          <t>Server226</t>
         </is>
       </c>
       <c r="C64">
-        <f>LOOKUP(2,1/(TorinoLocal!85:85&lt;&gt;""),TorinoLocal!85:85)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!97:97&lt;&gt;""),TransportsTresserras!97:97)</f>
         <v/>
       </c>
       <c r="D64">
-        <f>LOOKUP(2,1/(TorinoLocal!87:87&lt;&gt;""),TorinoLocal!87:87)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!99:99&lt;&gt;""),TransportsTresserras!99:99)</f>
         <v/>
       </c>
       <c r="E64">
-        <f>LOOKUP(2,1/(TorinoLocal!86:86&lt;&gt;""),TorinoLocal!86:86)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!98:98&lt;&gt;""),TransportsTresserras!98:98)</f>
         <v/>
       </c>
       <c r="F64" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>server251 - Unifi controller</t>
+          <t>Server227</t>
         </is>
       </c>
       <c r="C65">
-        <f>LOOKUP(2,1/(TorinoLocal!89:89&lt;&gt;""),TorinoLocal!89:89)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!101:101&lt;&gt;""),TransportsTresserras!101:101)</f>
         <v/>
       </c>
       <c r="D65">
-        <f>LOOKUP(2,1/(TorinoLocal!91:91&lt;&gt;""),TorinoLocal!91:91)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!103:103&lt;&gt;""),TransportsTresserras!103:103)</f>
         <v/>
       </c>
       <c r="E65">
-        <f>LOOKUP(2,1/(TorinoLocal!90:90&lt;&gt;""),TorinoLocal!90:90)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!102:102&lt;&gt;""),TransportsTresserras!102:102)</f>
         <v/>
       </c>
       <c r="F65" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>TorinoLocal</t>
+          <t>TransportsTresserras</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Server237 - SAPupdate (1)</t>
+          <t>Server235 - TS B1 Nou</t>
         </is>
       </c>
       <c r="C66">
-        <f>LOOKUP(2,1/(TorinoLocal!93:93&lt;&gt;""),TorinoLocal!93:93)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!105:105&lt;&gt;""),TransportsTresserras!105:105)</f>
         <v/>
       </c>
       <c r="D66">
-        <f>LOOKUP(2,1/(TorinoLocal!95:95&lt;&gt;""),TorinoLocal!95:95)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!107:107&lt;&gt;""),TransportsTresserras!107:107)</f>
         <v/>
       </c>
       <c r="E66">
-        <f>LOOKUP(2,1/(TorinoLocal!94:94&lt;&gt;""),TorinoLocal!94:94)</f>
+        <f>LOOKUP(2,1/(TransportsTresserras!106:106&lt;&gt;""),TransportsTresserras!106:106)</f>
         <v/>
       </c>
       <c r="F66" t="n">
-        <v>431</v>
+        <v>7177</v>
       </c>
     </row>
     <row r="67">
@@ -2664,13 +2660,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{461264EE-BDC7-472F-A751-2A60056AC369}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2E1603F-A0DD-4D88-8CE8-D8D686C3C1CB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39362BE3-EECB-44F8-B62C-A423C5606FA3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C493385E-9580-48B9-A813-A18ACBDA1EA5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FAC5AB1-5059-419F-B488-0D21E4A695CF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FF875E0-F565-4DA3-A069-C4794F4EBB5A}"/>
 </file>
</xml_diff>